<commit_message>
add suggested block to the Prac trialist
</commit_message>
<xml_diff>
--- a/trials/Prac_trial_list.xlsx
+++ b/trials/Prac_trial_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bsliang_Coganlabcode\Retrocue_taskscripts\trials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2D0DEC-4100-4E10-80C3-1F897286D989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B5046C-2AC5-4B61-B97C-34E5E02B2FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12852" yWindow="4620" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="16">
   <si>
     <t>Trial</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>REP_BTH</t>
+  </si>
+  <si>
+    <t>Suggested_Block</t>
   </si>
 </sst>
 </file>
@@ -427,15 +430,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -443,22 +446,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -468,20 +474,23 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.93883237807831976</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -491,20 +500,23 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.16407849330263111</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -514,20 +526,23 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.96531375757640525</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -537,20 +552,23 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
         <v>9</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.86825515328625247</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -560,20 +578,23 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
         <v>9</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.58491695984147807</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -583,20 +604,23 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
         <v>9</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.52634114140931265</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -606,20 +630,23 @@
       <c r="C8">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
-        <v>7</v>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
         <v>12</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>0.76297061886302542</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -629,20 +656,23 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.90557721296727056</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -652,20 +682,23 @@
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>0.93750773694932166</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -675,20 +708,23 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
-        <v>7</v>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
         <v>13</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.87730197039191837</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -698,20 +734,23 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
-        <v>8</v>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
         <v>13</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>0.47603943128551668</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -721,20 +760,23 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
-        <v>7</v>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
         <v>13</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>0.84650505808650944</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -744,20 +786,23 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
-        <v>8</v>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
         <v>11</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>0.23498626141125289</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -767,20 +812,23 @@
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
-        <v>7</v>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
         <v>11</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>0.2259775307707752</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -790,20 +838,23 @@
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
         <v>11</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>0.11317427819332999</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -813,20 +864,23 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
-        <v>7</v>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
         <v>14</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>0.90740179110665908</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -836,20 +890,23 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
-        <v>8</v>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
         <v>9</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>0.3897616093594426</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -859,20 +916,23 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" t="s">
-        <v>8</v>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
         <v>12</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>0.74204303195305488</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -882,20 +942,23 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
-        <v>10</v>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="s">
         <v>13</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>0.79865451073397631</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -905,16 +968,19 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" t="s">
-        <v>7</v>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="s">
         <v>11</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>0.13023073197723109</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change the practice session
</commit_message>
<xml_diff>
--- a/trials/Prac_trial_list.xlsx
+++ b/trials/Prac_trial_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bsliang_Coganlabcode\Retrocue_taskscripts\trials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B5046C-2AC5-4B61-B97C-34E5E02B2FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D613C40-DF7F-45F3-809E-0503C7C54E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12852" yWindow="4620" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +562,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H5">
         <v>0.86825515328625247</v>
@@ -588,7 +588,7 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H6">
         <v>0.58491695984147807</v>
@@ -614,7 +614,7 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H7">
         <v>0.52634114140931265</v>
@@ -640,7 +640,7 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H8">
         <v>0.76297061886302542</v>
@@ -666,7 +666,7 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H9">
         <v>0.90557721296727056</v>
@@ -692,7 +692,7 @@
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H10">
         <v>0.93750773694932166</v>
@@ -718,7 +718,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H11">
         <v>0.87730197039191837</v>
@@ -744,7 +744,7 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H12">
         <v>0.47603943128551668</v>
@@ -770,7 +770,7 @@
         <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H13">
         <v>0.84650505808650944</v>
@@ -900,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H18">
         <v>0.3897616093594426</v>
@@ -926,7 +926,7 @@
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H19">
         <v>0.74204303195305488</v>
@@ -952,7 +952,7 @@
         <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H20">
         <v>0.79865451073397631</v>

</xml_diff>

<commit_message>
Changed the instruction and task script input parameter strategy
</commit_message>
<xml_diff>
--- a/trials/Prac_trial_list.xlsx
+++ b/trials/Prac_trial_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bsliang_Coganlabcode\Retrocue_taskscripts\trials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D613C40-DF7F-45F3-809E-0503C7C54E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA05225-468F-4E24-9290-7536DE952E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12852" yWindow="4620" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,10 +433,19 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -487,7 +496,7 @@
         <v>14</v>
       </c>
       <c r="H2">
-        <v>0.93883237807831976</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -513,7 +522,7 @@
         <v>14</v>
       </c>
       <c r="H3">
-        <v>0.16407849330263111</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -539,7 +548,7 @@
         <v>14</v>
       </c>
       <c r="H4">
-        <v>0.96531375757640525</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -565,7 +574,7 @@
         <v>12</v>
       </c>
       <c r="H5">
-        <v>0.86825515328625247</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -591,7 +600,7 @@
         <v>12</v>
       </c>
       <c r="H6">
-        <v>0.58491695984147807</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -617,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="H7">
-        <v>0.52634114140931265</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -643,7 +652,7 @@
         <v>13</v>
       </c>
       <c r="H8">
-        <v>0.76297061886302542</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -669,7 +678,7 @@
         <v>13</v>
       </c>
       <c r="H9">
-        <v>0.90557721296727056</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -695,7 +704,7 @@
         <v>13</v>
       </c>
       <c r="H10">
-        <v>0.93750773694932166</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -721,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="H11">
-        <v>0.87730197039191837</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -747,7 +756,7 @@
         <v>9</v>
       </c>
       <c r="H12">
-        <v>0.47603943128551668</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -773,7 +782,7 @@
         <v>9</v>
       </c>
       <c r="H13">
-        <v>0.84650505808650944</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -799,7 +808,7 @@
         <v>11</v>
       </c>
       <c r="H14">
-        <v>0.23498626141125289</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -825,7 +834,7 @@
         <v>11</v>
       </c>
       <c r="H15">
-        <v>0.2259775307707752</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -851,7 +860,7 @@
         <v>11</v>
       </c>
       <c r="H16">
-        <v>0.11317427819332999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -877,7 +886,7 @@
         <v>14</v>
       </c>
       <c r="H17">
-        <v>0.90740179110665908</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -903,7 +912,7 @@
         <v>12</v>
       </c>
       <c r="H18">
-        <v>0.3897616093594426</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -929,7 +938,7 @@
         <v>13</v>
       </c>
       <c r="H19">
-        <v>0.74204303195305488</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -955,7 +964,7 @@
         <v>9</v>
       </c>
       <c r="H20">
-        <v>0.79865451073397631</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -981,7 +990,7 @@
         <v>11</v>
       </c>
       <c r="H21">
-        <v>0.13023073197723109</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>